<commit_message>
Inclusao de campos na secao de imovel do arquivo de envio para o dispositivo movel
</commit_message>
<xml_diff>
--- a/recadastramento/layout/Layout_Envio.xlsx
+++ b/recadastramento/layout/Layout_Envio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="24540" windowHeight="15540" tabRatio="948" activeTab="5"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="24540" windowHeight="15540" tabRatio="948" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cliente" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="185">
   <si>
     <t>linha tipo 01</t>
   </si>
@@ -530,13 +530,73 @@
   </si>
   <si>
     <t>linha tipo 17</t>
+  </si>
+  <si>
+    <t>area_construida</t>
+  </si>
+  <si>
+    <t>classe_social</t>
+  </si>
+  <si>
+    <t>quantidade_animais_domesticos</t>
+  </si>
+  <si>
+    <t>vol_cisterna</t>
+  </si>
+  <si>
+    <t>vol_piscina</t>
+  </si>
+  <si>
+    <t>vol_cx_dagua</t>
+  </si>
+  <si>
+    <t>tipo_uso</t>
+  </si>
+  <si>
+    <t>acesso_hidrometro</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>0 - Alta | 1 - Media | 2 - Baixa | 3 - Sub</t>
+  </si>
+  <si>
+    <t>0 - dormitorio | 1 - morada | 2 - veraneio | 3 - outros</t>
+  </si>
+  <si>
+    <t>0 - bom | 1 - ruim | 2 - sem</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Crianças</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Adultos</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Idosos</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Empregados</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Alunos</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Cães</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Outros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -599,8 +659,24 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,6 +693,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -644,10 +726,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -677,8 +771,27 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1078,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2579,16 +2692,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H38"/>
+  <dimension ref="B1:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.1640625" bestFit="1" customWidth="1"/>
@@ -2655,7 +2768,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" ref="D5:D38" si="0">SUM(C4,D4)</f>
+        <f t="shared" ref="D5:D53" si="0">SUM(C4,D4)</f>
         <v>12</v>
       </c>
       <c r="E5" s="5"/>
@@ -3194,9 +3307,263 @@
         <v>103</v>
       </c>
     </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" s="20">
+        <v>10</v>
+      </c>
+      <c r="D39" s="20">
+        <f t="shared" si="0"/>
+        <v>306</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" s="21">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" s="20">
+        <v>1</v>
+      </c>
+      <c r="D40" s="20">
+        <f t="shared" si="0"/>
+        <v>316</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="20">
+        <v>4</v>
+      </c>
+      <c r="D41" s="20">
+        <f t="shared" si="0"/>
+        <v>317</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="19"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="20">
+        <v>7</v>
+      </c>
+      <c r="D42" s="20">
+        <f t="shared" si="0"/>
+        <v>321</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F42" s="21">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43" s="20">
+        <v>7</v>
+      </c>
+      <c r="D43" s="20">
+        <f t="shared" si="0"/>
+        <v>328</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F43" s="21">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="20">
+        <v>7</v>
+      </c>
+      <c r="D44" s="20">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F44" s="21">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="20">
+        <v>1</v>
+      </c>
+      <c r="D45" s="20">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C46" s="20">
+        <v>1</v>
+      </c>
+      <c r="D46" s="20">
+        <f t="shared" si="0"/>
+        <v>343</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" s="20">
+        <v>4</v>
+      </c>
+      <c r="D47" s="20">
+        <f t="shared" si="0"/>
+        <v>344</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="19"/>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" s="20">
+        <v>4</v>
+      </c>
+      <c r="D48" s="20">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="19"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" s="20">
+        <v>4</v>
+      </c>
+      <c r="D49" s="20">
+        <f t="shared" si="0"/>
+        <v>352</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="19"/>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" s="20">
+        <v>4</v>
+      </c>
+      <c r="D50" s="20">
+        <f t="shared" si="0"/>
+        <v>356</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="19"/>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="20">
+        <v>4</v>
+      </c>
+      <c r="D51" s="20">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="19"/>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" s="20">
+        <v>4</v>
+      </c>
+      <c r="D52" s="20">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="19"/>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" s="20">
+        <v>4</v>
+      </c>
+      <c r="D53" s="20">
+        <f t="shared" si="0"/>
+        <v>368</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3543,7 +3910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mudanca de valores basicos das colunas de tipificacao de imovel.
Sao elas:
. classe social
. tipo de uso
. acesso de hidrometro
</commit_message>
<xml_diff>
--- a/recadastramento/layout/Layout_Envio.xlsx
+++ b/recadastramento/layout/Layout_Envio.xlsx
@@ -25,7 +25,7 @@
     <sheet name="Lista Capacidade Hidrometro" sheetId="16" r:id="rId16"/>
     <sheet name="Lista Tipo Logradouro" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -562,15 +562,6 @@
     <t>Short</t>
   </si>
   <si>
-    <t>0 - Alta | 1 - Media | 2 - Baixa | 3 - Sub</t>
-  </si>
-  <si>
-    <t>0 - dormitorio | 1 - morada | 2 - veraneio | 3 - outros</t>
-  </si>
-  <si>
-    <t>0 - bom | 1 - ruim | 2 - sem</t>
-  </si>
-  <si>
     <t>Tipo de ocupante: Crianças</t>
   </si>
   <si>
@@ -590,6 +581,15 @@
   </si>
   <si>
     <t>Tipo de ocupante: Outros</t>
+  </si>
+  <si>
+    <t>1 - Alta | 2 - Media | 3 - Baixa | 4 - Sub</t>
+  </si>
+  <si>
+    <t>1 - dormitorio | 2 - morada | 3 - veraneio | 4 - outros</t>
+  </si>
+  <si>
+    <t>1 - bom | 2 - ruim | 3 - sem</t>
   </si>
 </sst>
 </file>
@@ -2694,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3340,7 +3340,7 @@
         <v>174</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="2:8">
@@ -3428,7 +3428,7 @@
         <v>174</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -3446,12 +3446,12 @@
         <v>174</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C47" s="20">
         <v>4</v>
@@ -3467,7 +3467,7 @@
     </row>
     <row r="48" spans="2:8">
       <c r="B48" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C48" s="20">
         <v>4</v>
@@ -3483,7 +3483,7 @@
     </row>
     <row r="49" spans="2:6">
       <c r="B49" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C49" s="20">
         <v>4</v>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="50" spans="2:6">
       <c r="B50" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C50" s="20">
         <v>4</v>
@@ -3515,7 +3515,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C51" s="20">
         <v>4</v>
@@ -3531,7 +3531,7 @@
     </row>
     <row r="52" spans="2:6">
       <c r="B52" s="19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C52" s="20">
         <v>4</v>
@@ -3547,7 +3547,7 @@
     </row>
     <row r="53" spans="2:6">
       <c r="B53" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C53" s="20">
         <v>4</v>

</xml_diff>

<commit_message>
Novas categorias no arquivo da atualizacao cadastral
Foram criadas as linhas:
. 18 - classe social
. 19 - Tipo de uso do imovel
. 20 - Acesso ao hidrometro
</commit_message>
<xml_diff>
--- a/recadastramento/layout/Layout_Envio.xlsx
+++ b/recadastramento/layout/Layout_Envio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="24540" windowHeight="15540" tabRatio="948" activeTab="1"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="24540" windowHeight="15540" tabRatio="948" firstSheet="14" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Cliente" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,9 @@
     <sheet name="Lista Local Instalacao Ramal" sheetId="15" r:id="rId15"/>
     <sheet name="Lista Capacidade Hidrometro" sheetId="16" r:id="rId16"/>
     <sheet name="Lista Tipo Logradouro" sheetId="17" r:id="rId17"/>
+    <sheet name="Lista Classe Social" sheetId="18" r:id="rId18"/>
+    <sheet name="Lista Tipo de Uso do Imovel" sheetId="19" r:id="rId19"/>
+    <sheet name="Lista Acesso ao Hridrometro" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="188">
   <si>
     <t>linha tipo 01</t>
   </si>
@@ -590,6 +593,15 @@
   </si>
   <si>
     <t>1 - bom | 2 - ruim | 3 - sem</t>
+  </si>
+  <si>
+    <t>linha tipo 18</t>
+  </si>
+  <si>
+    <t>linha tipo 19</t>
+  </si>
+  <si>
+    <t>linha tipo 20</t>
   </si>
 </sst>
 </file>
@@ -726,8 +738,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -779,19 +799,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2613,7 +2641,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2681,7 +2709,171 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23">
+      <c r="A1" s="18"/>
+      <c r="B1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A3" s="18"/>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A4" s="18"/>
+      <c r="B4" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="13">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23">
+      <c r="A1" s="18"/>
+      <c r="B1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A3" s="18"/>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A4" s="18"/>
+      <c r="B4" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="13">
+        <v>20</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2694,7 +2886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
@@ -3564,6 +3756,87 @@
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23">
+      <c r="A1" s="18"/>
+      <c r="B1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A3" s="18"/>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A4" s="18"/>
+      <c r="B4" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="17.75" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="13">
+        <v>20</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Novos valores para a linha de imovel.
Foram inseridas:
. quantidade de economias para a categoria social
. quantidade de economias para outra categoria
</commit_message>
<xml_diff>
--- a/recadastramento/layout/Layout_Envio.xlsx
+++ b/recadastramento/layout/Layout_Envio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="24540" windowHeight="15540" tabRatio="948" firstSheet="14" activeTab="19"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="24580" windowHeight="15540" tabRatio="948" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cliente" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="190">
   <si>
     <t>linha tipo 01</t>
   </si>
@@ -602,6 +602,12 @@
   </si>
   <si>
     <t>linha tipo 20</t>
+  </si>
+  <si>
+    <t>quantidade_economias_social</t>
+  </si>
+  <si>
+    <t>quantidade_economias_outros</t>
   </si>
 </sst>
 </file>
@@ -738,8 +744,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -799,7 +807,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -810,6 +818,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -820,6 +829,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2884,17 +2894,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H53"/>
+  <dimension ref="B1:H55"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2960,7 +2970,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" ref="D5:D53" si="0">SUM(C4,D4)</f>
+        <f t="shared" ref="D5:D55" si="0">SUM(C4,D4)</f>
         <v>12</v>
       </c>
       <c r="E5" s="5"/>
@@ -3673,7 +3683,7 @@
       </c>
       <c r="F48" s="19"/>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:8">
       <c r="B49" s="19" t="s">
         <v>177</v>
       </c>
@@ -3689,7 +3699,7 @@
       </c>
       <c r="F49" s="19"/>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:8">
       <c r="B50" s="19" t="s">
         <v>178</v>
       </c>
@@ -3705,7 +3715,7 @@
       </c>
       <c r="F50" s="19"/>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:8">
       <c r="B51" s="19" t="s">
         <v>179</v>
       </c>
@@ -3721,7 +3731,7 @@
       </c>
       <c r="F51" s="19"/>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:8">
       <c r="B52" s="19" t="s">
         <v>180</v>
       </c>
@@ -3737,7 +3747,7 @@
       </c>
       <c r="F52" s="19"/>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:8">
       <c r="B53" s="19" t="s">
         <v>181</v>
       </c>
@@ -3752,6 +3762,40 @@
         <v>9</v>
       </c>
       <c r="F53" s="19"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54" s="20">
+        <v>3</v>
+      </c>
+      <c r="D54" s="20">
+        <f t="shared" si="0"/>
+        <v>372</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="19"/>
+      <c r="H54" s="14"/>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C55" s="20">
+        <v>3</v>
+      </c>
+      <c r="D55" s="20">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="19"/>
+      <c r="H55" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3768,7 +3812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>